<commit_message>
update status of bugs: 1,2,3,4
</commit_message>
<xml_diff>
--- a/04_TESTING/Leakage_Bug_List.xlsx
+++ b/04_TESTING/Leakage_Bug_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="3030" windowWidth="20730" windowHeight="7245" tabRatio="726"/>
+    <workbookView xWindow="60" yWindow="3030" windowWidth="20610" windowHeight="7245" tabRatio="726"/>
   </bookViews>
   <sheets>
     <sheet name="Leakage Bug List" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="91">
   <si>
     <t>Leakage ID</t>
   </si>
@@ -5805,12 +5805,25 @@
       <t xml:space="preserve"> Hiển thị câu thông báo Region Name đã tồn tại</t>
     </r>
   </si>
+  <si>
+    <t>Dev Status</t>
+  </si>
+  <si>
+    <t>Dev Note</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>- Fixed
+Tuy nhien khi tao moi the Customer co flag IsEnabled = false nen se ko hien thi duoc tren Grid Cusromer, ma` phai approve o cai Grid ben duoi moi co the view duoc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5877,8 +5890,16 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5894,6 +5915,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5959,7 +5986,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5999,6 +6026,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6591,12 +6639,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G63"/>
+  <dimension ref="B2:I63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6608,23 +6656,26 @@
     <col min="5" max="5" width="16.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="13" style="5" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="4.85546875" style="5"/>
+    <col min="8" max="9" width="24.28515625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="4.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -6643,8 +6694,14 @@
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="5" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -6661,8 +6718,14 @@
       <c r="G5" s="8" t="s">
         <v>68</v>
       </c>
+      <c r="H5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -6679,8 +6742,12 @@
         <v>17</v>
       </c>
       <c r="G6" s="8"/>
+      <c r="H6" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -6695,8 +6762,12 @@
         <v>17</v>
       </c>
       <c r="G7" s="8"/>
+      <c r="H7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -6713,8 +6784,12 @@
         <v>17</v>
       </c>
       <c r="G8" s="8"/>
+      <c r="H8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>5</v>
       </c>
@@ -6731,8 +6806,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="8"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -6747,8 +6824,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="8"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
@@ -6763,8 +6842,10 @@
         <v>17</v>
       </c>
       <c r="G11" s="8"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -6779,8 +6860,10 @@
         <v>17</v>
       </c>
       <c r="G12" s="8"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -6795,8 +6878,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="8"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>10</v>
       </c>
@@ -6813,8 +6898,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="8"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>11</v>
       </c>
@@ -6829,8 +6916,10 @@
         <v>17</v>
       </c>
       <c r="G15" s="8"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>12</v>
       </c>
@@ -6845,8 +6934,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="8"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="2:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="240" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>13</v>
       </c>
@@ -6863,8 +6954,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="8"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>14</v>
       </c>
@@ -6879,8 +6972,10 @@
         <v>17</v>
       </c>
       <c r="G18" s="8"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -6895,8 +6990,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="8"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>16</v>
       </c>
@@ -6911,8 +7008,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="8"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>17</v>
       </c>
@@ -6927,8 +7026,10 @@
         <v>17</v>
       </c>
       <c r="G21" s="8"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>18</v>
       </c>
@@ -6943,8 +7044,10 @@
         <v>17</v>
       </c>
       <c r="G22" s="8"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>19</v>
       </c>
@@ -6959,8 +7062,10 @@
         <v>17</v>
       </c>
       <c r="G23" s="8"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>20</v>
       </c>
@@ -6975,8 +7080,10 @@
         <v>17</v>
       </c>
       <c r="G24" s="8"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="2:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="315" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>21</v>
       </c>
@@ -6991,8 +7098,10 @@
         <v>17</v>
       </c>
       <c r="G25" s="8"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>22</v>
       </c>
@@ -7007,8 +7116,10 @@
         <v>17</v>
       </c>
       <c r="G26" s="8"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>23</v>
       </c>
@@ -7023,8 +7134,10 @@
         <v>17</v>
       </c>
       <c r="G27" s="8"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="2:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="360" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>24</v>
       </c>
@@ -7039,8 +7152,10 @@
         <v>17</v>
       </c>
       <c r="G28" s="8"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="2:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="315" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>25</v>
       </c>
@@ -7055,8 +7170,10 @@
         <v>17</v>
       </c>
       <c r="G29" s="8"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>26</v>
       </c>
@@ -7073,8 +7190,10 @@
       <c r="G30" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="H30" s="19"/>
+      <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>27</v>
       </c>
@@ -7089,8 +7208,10 @@
         <v>17</v>
       </c>
       <c r="G31" s="8"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>28</v>
       </c>
@@ -7105,8 +7226,10 @@
         <v>17</v>
       </c>
       <c r="G32" s="8"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>29</v>
       </c>
@@ -7121,8 +7244,10 @@
         <v>17</v>
       </c>
       <c r="G33" s="8"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="2:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="255" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>30</v>
       </c>
@@ -7137,8 +7262,10 @@
         <v>17</v>
       </c>
       <c r="G34" s="8"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>31</v>
       </c>
@@ -7153,8 +7280,10 @@
         <v>17</v>
       </c>
       <c r="G35" s="8"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="2:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="240" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>32</v>
       </c>
@@ -7169,8 +7298,10 @@
         <v>17</v>
       </c>
       <c r="G36" s="8"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="2:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="240" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>33</v>
       </c>
@@ -7185,8 +7316,10 @@
         <v>17</v>
       </c>
       <c r="G37" s="8"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="2:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="210" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>34</v>
       </c>
@@ -7201,8 +7334,10 @@
         <v>17</v>
       </c>
       <c r="G38" s="8"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="2:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="240" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>35</v>
       </c>
@@ -7217,8 +7352,10 @@
         <v>17</v>
       </c>
       <c r="G39" s="8"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>36</v>
       </c>
@@ -7233,8 +7370,10 @@
         <v>17</v>
       </c>
       <c r="G40" s="8"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>37</v>
       </c>
@@ -7249,8 +7388,10 @@
         <v>17</v>
       </c>
       <c r="G41" s="8"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>38</v>
       </c>
@@ -7267,8 +7408,10 @@
       <c r="G42" s="8" t="s">
         <v>69</v>
       </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>39</v>
       </c>
@@ -7284,7 +7427,7 @@
       </c>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>40</v>
       </c>
@@ -7300,7 +7443,7 @@
       </c>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" ht="180" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>41</v>
       </c>
@@ -7316,7 +7459,7 @@
       </c>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>42</v>
       </c>
@@ -7332,7 +7475,7 @@
       </c>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="2:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" ht="255" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>43</v>
       </c>
@@ -7348,7 +7491,7 @@
       </c>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" ht="195" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
add new and update bug
</commit_message>
<xml_diff>
--- a/04_TESTING/Leakage_Bug_List.xlsx
+++ b/04_TESTING/Leakage_Bug_List.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="181">
   <si>
     <t>Leakage ID</t>
   </si>
@@ -3587,100 +3587,6 @@
       <t xml:space="preserve"> 
        1. Chưa chọn ngày thì ngày hiện tại phải được highlight
        2. Chọn ngày thì ngày được chọn phải highlight</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong Filter chọn customer, salemen hoặc Administrator
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Repro:
-  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 1. Login vào Account của Salesmen/Customer/Administrator
-   2. Click vào SMS List  trên menu
-   3. Click vào Compose button
-   4. Click vào "Browse" button
-   5. Trong Form Filter lần lượt chọn value trong Group  &gt; Region &gt; Area &gt; Local
-    6. Click chọn value là "Select a type" trong Group hay Region</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-       Chỉ reset lại cấp con của nó
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-      Phải reset lại hết các cấp dưới
-(VD: 6. chọn Value là 'Select a type' trong Group" thì các Field Region + Area + local phải được reset mà không phải chỉ reset lại Field Region không)</t>
     </r>
   </si>
   <si>
@@ -9858,340 +9764,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Hiển thị title của Tab Browser không đúng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Repro: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">     - Login vào account của Administrator</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. Click vào Inbox trong SMS List
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Dashboard"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Inbox"
-       2. Click vào Failure trong SMS List
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/SMSFailure.aspx"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Failure"
-      3. Click vào Compose button
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị URL "http://pharma.u-matrixsoft.com/Administrator/ComposeSMS.aspx"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "Compose SMS"
-      4. Click vào Administrator &gt;&gt; SMS &amp; Customer Data &gt;&gt; Allow Approve
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Ko thay muc Allow Approve in SMS &amp; Customer data, chi thay muc Allow Approve in Permission =&gt; sua muc do
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tam] okie anh do em ghi sai</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/AllowApprove.aspx"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "Allow Approve"
-       5. Click vào Administrator &gt;&gt; SMS &amp; Customer Data &gt;&gt; SMS Type
- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/SmsTypeManagement.aspx"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Type"</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lỗi trong chức năng Update
 </t>
     </r>
@@ -10522,37 +10094,6 @@
   </si>
   <si>
     <t xml:space="preserve">Administrator &gt;&gt; Permission &gt;&gt; Allow Approve </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Khi click vào button Browser chọn Phone number sẽ hiển thị ra </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Select phone number
-[Dan] Em co the mo ta tu` luc login vao den luc xay ra bug duoc ko? Thanks
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tam]Okie anh, em đã mô tả lại, anh xem và fixed hộ em nhé</t>
-    </r>
   </si>
   <si>
     <r>
@@ -12538,6 +12079,576 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">     Hiện record sms vừa gửi, nhưng cột FROM phải GET lên tên của người gửi</t>
+    </r>
+  </si>
+  <si>
+    <t>[Tam - 28/05/2012] vậy sao không thêm điều kiện khi get "phone number (1)"
+- phone number (1) sẽ hiển thị theo điều kiện là chỉ count những số phone nào được chọn và hiện tại đang tồn tại -&gt; để khi User xem chi tiet nó thống nhất về con số được count hơn</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong Filter chọn customer, salemen hoặc Administrator
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Repro:
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1. Login vào Account của Salesmen/Administrator
+   2. Click vào SMS List  trên menu
+   3. Click vào Compose button
+   4. Click vào "Browse" button
+   5. Trong Form Filter lần lượt chọn value trong Group  &gt; Region &gt; Area &gt; Local
+    6. Click chọn value là "Select a type" trong Group hay Region</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+       Chỉ reset lại cấp con của nó
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      Phải reset lại hết các cấp dưới
+(VD: 6. chọn Value là 'Select a type' trong Group" thì các Field Region + Area + local phải được reset mà không phải chỉ reset lại Field Region không)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Khi click vào button Browser chọn Phone number sẽ hiển thị ra </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Select phone number
+[Dan] Em co the mo ta tu` luc login vao den luc xay ra bug duoc ko? Thanks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tam]Okie anh, em đã mô tả lại, anh xem và fixed hộ em nhé
+[Tâm] retest 28/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hiển thị title của Tab Browser không đúng
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Repro: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     - Login vào account của Administrator</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Click vào Inbox trong SMS List
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Dashboard"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Inbox"
+       2. Click vào Failure trong SMS List
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/SMSFailure.aspx"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Failure"
+      3. Click vào Compose button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị URL "http://pharma.u-matrixsoft.com/Administrator/ComposeSMS.aspx"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "Compose SMS"
+      4. Click vào Administrator &gt;&gt; Permission &gt;&gt; Allow Approve
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Ko thay muc Allow Approve in SMS &amp; Customer data, chi thay muc Allow Approve in Permission =&gt; sua muc do
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tam] okie anh do em ghi sai, đã sửa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/AllowApprove.aspx"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "Allow Approve"
+       5. Click vào Administrator &gt;&gt; SMS &amp; Customer Data &gt;&gt; SMS Type
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Trên tab Browser hiển thị  URL "http://pharma.u-matrixsoft.com/Administrator/SmsTypeManagement.aspx"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trên tab Browser hiển thị "SMS Type"</t>
+    </r>
+  </si>
+  <si>
+    <t>[Tâm] retest 28/5/2012 - Passed
+Nhưng case  3. Nhập vào Name với giá trị đã tồn tại hiện thông báo khó hiểu " Can not add, please provide new name or try again or contact administrator! "
+--&gt; có thể thông báo "giá trị đã tồn tại, vui lòng nhập tên khác" vì hiện tại đang dùng account của administrator thì không cần câu "or contact administrator! "</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click vào icon cancel thì không đóng form Add new
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repro:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    - Login vào Account của Administrator
+    - Click vào Administrator trên menu
+    - Click vào Permistion &gt;&gt; Role bên trái
+    - Click mở Form Add New Record
+    -  Click vào icon "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cancel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Không đóng Form Add new
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Đóng Form Add new</t>
     </r>
   </si>
 </sst>
@@ -12878,7 +12989,63 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -13666,9 +13833,9 @@
   <dimension ref="B2:I108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13679,7 +13846,7 @@
     <col min="4" max="4" width="81" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="13" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="5" customWidth="1"/>
     <col min="8" max="9" width="24.28515625" style="4" customWidth="1"/>
     <col min="10" max="16384" width="4.85546875" style="4"/>
   </cols>
@@ -13738,10 +13905,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>58</v>
@@ -13765,10 +13932,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>58</v>
@@ -13788,10 +13955,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>58</v>
@@ -13813,10 +13980,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>58</v>
@@ -13832,16 +13999,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>58</v>
@@ -13861,10 +14028,10 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>58</v>
@@ -13887,7 +14054,7 @@
         <v>17</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>62</v>
@@ -13907,10 +14074,10 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>63</v>
@@ -13930,10 +14097,10 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>58</v>
@@ -13972,14 +14139,14 @@
         <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>58</v>
@@ -13999,9 +14166,11 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H16" s="13" t="s">
         <v>58</v>
       </c>
@@ -14024,7 +14193,9 @@
       <c r="F17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="20" t="s">
+        <v>175</v>
+      </c>
       <c r="H17" s="13" t="s">
         <v>58</v>
       </c>
@@ -14045,9 +14216,11 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H18" s="13" t="s">
         <v>58</v>
       </c>
@@ -14062,14 +14235,14 @@
         <v>8</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="23" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>58</v>
@@ -14089,9 +14262,11 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H20" s="13" t="s">
         <v>58</v>
       </c>
@@ -14110,9 +14285,11 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H21" s="13" t="s">
         <v>58</v>
       </c>
@@ -14131,9 +14308,11 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H22" s="13" t="s">
         <v>58</v>
       </c>
@@ -14152,9 +14331,11 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H23" s="13" t="s">
         <v>58</v>
       </c>
@@ -14173,9 +14354,11 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H24" s="13" t="s">
         <v>58</v>
       </c>
@@ -14190,13 +14373,15 @@
         <v>22</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H25" s="13" t="s">
         <v>58</v>
       </c>
@@ -14211,13 +14396,15 @@
         <v>43</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="7"/>
+      <c r="G26" s="20" t="s">
+        <v>179</v>
+      </c>
       <c r="H26" s="13" t="s">
         <v>58</v>
       </c>
@@ -14232,7 +14419,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2" t="s">
@@ -14253,7 +14440,7 @@
         <v>44</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2" t="s">
@@ -14274,7 +14461,7 @@
         <v>44</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="2" t="s">
@@ -14292,17 +14479,17 @@
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>58</v>
@@ -14318,7 +14505,7 @@
         <v>45</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="2" t="s">
@@ -14339,7 +14526,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="2" t="s">
@@ -14360,7 +14547,7 @@
         <v>47</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="2" t="s">
@@ -14381,7 +14568,7 @@
         <v>47</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2" t="s">
@@ -14402,7 +14589,7 @@
         <v>48</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="2" t="s">
@@ -14423,7 +14610,7 @@
         <v>48</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2" t="s">
@@ -14444,7 +14631,7 @@
         <v>48</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="2" t="s">
@@ -14465,7 +14652,7 @@
         <v>49</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="2" t="s">
@@ -14486,7 +14673,7 @@
         <v>49</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2" t="s">
@@ -14507,7 +14694,7 @@
         <v>50</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="2" t="s">
@@ -14528,7 +14715,7 @@
         <v>50</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="2" t="s">
@@ -14549,7 +14736,7 @@
         <v>51</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="2" t="s">
@@ -14572,7 +14759,7 @@
         <v>51</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
@@ -14592,7 +14779,7 @@
         <v>53</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
@@ -14612,7 +14799,7 @@
         <v>53</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
@@ -14632,7 +14819,7 @@
         <v>54</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
@@ -14652,7 +14839,7 @@
         <v>54</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
@@ -14672,7 +14859,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
@@ -14692,7 +14879,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
@@ -14712,7 +14899,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
@@ -14732,7 +14919,7 @@
         <v>60</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
@@ -14752,7 +14939,7 @@
         <v>61</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
@@ -14772,7 +14959,7 @@
         <v>61</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
@@ -14812,7 +14999,7 @@
         <v>65</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
@@ -14820,7 +15007,7 @@
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="150" x14ac:dyDescent="0.25">
@@ -14914,7 +15101,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="120" x14ac:dyDescent="0.25">
@@ -14933,10 +15120,10 @@
         <v>17</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H61" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="180" x14ac:dyDescent="0.25">
@@ -14956,7 +15143,7 @@
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="2:8" ht="210" x14ac:dyDescent="0.25">
@@ -14974,7 +15161,7 @@
       <c r="F63" s="2"/>
       <c r="G63" s="7"/>
       <c r="H63" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="195" x14ac:dyDescent="0.25">
@@ -14993,10 +15180,10 @@
         <v>17</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="2:8" ht="210" x14ac:dyDescent="0.25">
@@ -15015,10 +15202,10 @@
         <v>17</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15038,7 +15225,7 @@
       </c>
       <c r="G66" s="7"/>
       <c r="H66" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="2:8" ht="150" x14ac:dyDescent="0.25">
@@ -15058,7 +15245,7 @@
       </c>
       <c r="G67" s="7"/>
       <c r="H67" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="180" x14ac:dyDescent="0.25">
@@ -15078,7 +15265,7 @@
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15098,7 +15285,7 @@
       </c>
       <c r="G69" s="7"/>
       <c r="H69" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15127,7 +15314,7 @@
         <v>89</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
@@ -15135,7 +15322,7 @@
       </c>
       <c r="G71" s="7"/>
       <c r="H71" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15154,7 +15341,7 @@
         <v>17</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="195" x14ac:dyDescent="0.25">
@@ -15191,7 +15378,7 @@
       </c>
       <c r="G74" s="7"/>
       <c r="H74" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="2:8" ht="150" x14ac:dyDescent="0.25">
@@ -15207,13 +15394,13 @@
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15239,22 +15426,22 @@
         <v>73</v>
       </c>
       <c r="C77" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="E77" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="2:8" ht="210" x14ac:dyDescent="0.25">
@@ -15263,10 +15450,10 @@
         <v>74</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
@@ -15274,7 +15461,7 @@
       </c>
       <c r="G78" s="7"/>
       <c r="H78" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="2:8" ht="150" x14ac:dyDescent="0.25">
@@ -15283,10 +15470,10 @@
         <v>75</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
@@ -15294,7 +15481,7 @@
       </c>
       <c r="G79" s="7"/>
       <c r="H79" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="2:8" ht="225" x14ac:dyDescent="0.25">
@@ -15303,20 +15490,20 @@
         <v>76</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="2:8" ht="105" x14ac:dyDescent="0.25">
@@ -15325,10 +15512,10 @@
         <v>77</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2" t="s">
@@ -15336,7 +15523,7 @@
       </c>
       <c r="G81" s="7"/>
       <c r="H81" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="2:8" ht="120" x14ac:dyDescent="0.25">
@@ -15345,10 +15532,10 @@
         <v>78</v>
       </c>
       <c r="C82" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2" t="s">
@@ -15356,7 +15543,7 @@
       </c>
       <c r="G82" s="19"/>
       <c r="H82" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="240" x14ac:dyDescent="0.25">
@@ -15365,10 +15552,10 @@
         <v>79</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
@@ -15376,7 +15563,7 @@
       </c>
       <c r="G83" s="19"/>
       <c r="H83" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="2:8" ht="225" x14ac:dyDescent="0.25">
@@ -15385,10 +15572,10 @@
         <v>80</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2" t="s">
@@ -15396,7 +15583,7 @@
       </c>
       <c r="G84" s="19"/>
       <c r="H84" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15405,10 +15592,10 @@
         <v>81</v>
       </c>
       <c r="C85" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2" t="s">
@@ -15416,7 +15603,7 @@
       </c>
       <c r="G85" s="7"/>
       <c r="H85" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="2:8" ht="315" x14ac:dyDescent="0.25">
@@ -15425,10 +15612,10 @@
         <v>82</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
@@ -15436,7 +15623,7 @@
       </c>
       <c r="G86" s="7"/>
       <c r="H86" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="2:8" ht="195" x14ac:dyDescent="0.25">
@@ -15445,10 +15632,10 @@
         <v>83</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
@@ -15456,7 +15643,7 @@
       </c>
       <c r="G87" s="7"/>
       <c r="H87" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="2:8" ht="165" x14ac:dyDescent="0.25">
@@ -15465,20 +15652,20 @@
         <v>84</v>
       </c>
       <c r="C88" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="2:8" ht="135" x14ac:dyDescent="0.25">
@@ -15487,10 +15674,10 @@
         <v>85</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
@@ -15504,10 +15691,10 @@
         <v>86</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
@@ -15524,7 +15711,7 @@
         <v>7</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -15541,7 +15728,7 @@
         <v>18</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
@@ -15549,15 +15736,21 @@
       </c>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="str">
+    <row r="93" spans="2:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="B93" s="2">
         <f>IF(D93="","",MAX($B$4:$B92)+1)</f>
-        <v/>
-      </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>180</v>
+      </c>
       <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
+      <c r="F93" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G93" s="7"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -15728,7 +15921,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G200">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$F5="Close"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
explain why use the term "contact administrator"
</commit_message>
<xml_diff>
--- a/04_TESTING/Leakage_Bug_List.xlsx
+++ b/04_TESTING/Leakage_Bug_List.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Leakage Bug List'!$B$4:$G$107</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="211">
   <si>
     <t>Leakage ID</t>
   </si>
@@ -10999,11 +10999,6 @@
     </r>
   </si>
   <si>
-    <t>[Tâm] retest 28/5/2012 - Passed
-Nhưng case  3. Nhập vào Name với giá trị đã tồn tại hiện thông báo khó hiểu " Can not add, please provide new name or try again or contact administrator! "
---&gt; có thể thông báo "giá trị đã tồn tại, vui lòng nhập tên khác" vì hiện tại đang dùng account của administrator thì không cần câu "or contact administrator! "</t>
-  </si>
-  <si>
     <t>Administrator &gt;&gt; Permistion &gt;&gt; Administrator</t>
   </si>
   <si>
@@ -14052,6 +14047,19 @@
   <si>
     <t>[Tâm] retest 28/5/2012 - Failed
 can not update, please try again later or contact admnistrator. (tương tự bug 41)</t>
+  </si>
+  <si>
+    <t>[Tâm] retest 28/5/2012 - Passed
+Nhưng case  3. Nhập vào Name với giá trị đã tồn tại hiện thông báo khó hiểu " Can not add, please provide new name or try again or contact administrator! "
+--&gt; có thể thông báo "giá trị đã tồn tại, vui lòng nhập tên khác" vì hiện tại đang dùng account của administrator thì không cần câu "or contact administrator! "
+[Dan] Administrator o day la` nguoi quan tri cua web site, co`n logged user chi la` admin cua site thoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tâm] retest 28/5/2012 - Passed
+Nhưng case  3. Nhập vào Name với giá trị đã tồn tại hiện thông báo khó hiểu " Can not add, please provide new name or try again or contact administrator! "
+--&gt; có thể thông báo "giá trị đã tồn tại, vui lòng nhập tên khác" vì hiện tại đang dùng account của administrator thì không cần câu "or contact administrator! "
+[Dan] Administrator o day la` nguoi quan tri cua web site, co`n logged user chi la` admin cua site thoi
+</t>
   </si>
 </sst>
 </file>
@@ -14399,98 +14407,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -15177,12 +15094,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:I108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15242,7 +15160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <f>IF(D5="","",MAX($B$4:$B4)+1)</f>
         <v>1</v>
@@ -15267,7 +15185,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <f>IF(D6="","",MAX($B$4:$B5)+1)</f>
         <v>2</v>
@@ -15292,7 +15210,7 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="2:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <f>IF(D7="","",MAX($B$4:$B6)+1)</f>
         <v>3</v>
@@ -15315,7 +15233,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <f>IF(D8="","",MAX($B$4:$B7)+1)</f>
         <v>4</v>
@@ -15340,7 +15258,7 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <f>IF(D9="","",MAX($B$4:$B8)+1)</f>
         <v>5</v>
@@ -15365,7 +15283,7 @@
       </c>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f>IF(D10="","",MAX($B$4:$B9)+1)</f>
         <v>6</v>
@@ -15411,7 +15329,7 @@
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f>IF(D12="","",MAX($B$4:$B11)+1)</f>
         <v>8</v>
@@ -15434,7 +15352,7 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <f>IF(D13="","",MAX($B$4:$B12)+1)</f>
         <v>9</v>
@@ -15457,7 +15375,7 @@
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="2:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <f>IF(D14="","",MAX($B$4:$B13)+1)</f>
         <v>10</v>
@@ -15482,7 +15400,7 @@
       </c>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="2:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f>IF(D15="","",MAX($B$4:$B14)+1)</f>
         <v>11</v>
@@ -15505,7 +15423,7 @@
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="2:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <f>IF(D16="","",MAX($B$4:$B15)+1)</f>
         <v>12</v>
@@ -15555,7 +15473,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <f>IF(D18="","",MAX($B$4:$B17)+1)</f>
         <v>14</v>
@@ -15578,7 +15496,7 @@
       </c>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="2:9" s="27" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" s="27" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <f>IF(D19="","",MAX($B$4:$B18)+1)</f>
         <v>15</v>
@@ -15601,7 +15519,7 @@
       </c>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <f>IF(D20="","",MAX($B$4:$B19)+1)</f>
         <v>16</v>
@@ -15624,7 +15542,7 @@
       </c>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <f>IF(D21="","",MAX($B$4:$B20)+1)</f>
         <v>17</v>
@@ -15647,7 +15565,7 @@
       </c>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="2:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <f>IF(D22="","",MAX($B$4:$B21)+1)</f>
         <v>18</v>
@@ -15670,7 +15588,7 @@
       </c>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <f>IF(D23="","",MAX($B$4:$B22)+1)</f>
         <v>19</v>
@@ -15693,7 +15611,7 @@
       </c>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="2:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <f>IF(D24="","",MAX($B$4:$B23)+1)</f>
         <v>20</v>
@@ -15716,7 +15634,7 @@
       </c>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="2:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <f>IF(D25="","",MAX($B$4:$B24)+1)</f>
         <v>21</v>
@@ -15755,7 +15673,7 @@
         <v>17</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>56</v>
@@ -15778,7 +15696,7 @@
         <v>17</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>56</v>
@@ -15791,7 +15709,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>144</v>
@@ -15801,7 +15719,7 @@
         <v>17</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>56</v>
@@ -15814,7 +15732,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>140</v>
@@ -15824,14 +15742,14 @@
         <v>17</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <f>IF(D30="","",MAX($B$4:$B29)+1)</f>
         <v>26</v>
@@ -15870,7 +15788,7 @@
         <v>17</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>56</v>
@@ -15893,7 +15811,7 @@
         <v>17</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>56</v>
@@ -15916,7 +15834,7 @@
         <v>17</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>56</v>
@@ -15939,14 +15857,14 @@
         <v>17</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <f>IF(D35="","",MAX($B$4:$B34)+1)</f>
         <v>31</v>
@@ -15978,14 +15896,14 @@
         <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>56</v>
@@ -16008,7 +15926,7 @@
         <v>17</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>56</v>
@@ -16031,7 +15949,7 @@
         <v>17</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>56</v>
@@ -16054,7 +15972,7 @@
         <v>17</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>56</v>
@@ -16077,7 +15995,7 @@
         <v>17</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>56</v>
@@ -16100,7 +16018,7 @@
         <v>17</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>56</v>
@@ -16123,7 +16041,7 @@
         <v>17</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>56</v>
@@ -16146,7 +16064,7 @@
         <v>17</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>56</v>
@@ -16168,7 +16086,7 @@
         <v>17</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>56</v>
@@ -16190,7 +16108,7 @@
         <v>17</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>56</v>
@@ -16212,7 +16130,7 @@
         <v>17</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>56</v>
@@ -16234,7 +16152,7 @@
         <v>17</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>56</v>
@@ -16256,7 +16174,7 @@
         <v>17</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>56</v>
@@ -16278,7 +16196,7 @@
         <v>17</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>56</v>
@@ -16300,7 +16218,7 @@
         <v>17</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>56</v>
@@ -16322,7 +16240,7 @@
         <v>17</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>56</v>
@@ -16344,7 +16262,7 @@
         <v>17</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H52" s="13" t="s">
         <v>56</v>
@@ -16366,13 +16284,13 @@
         <v>17</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <f>IF(D54="","",MAX($B$4:$B53)+1)</f>
         <v>50</v>
@@ -16403,20 +16321,20 @@
         <v>63</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H55" s="29" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <f>IF(D56="","",MAX($B$4:$B55)+1)</f>
         <v>52</v>
@@ -16438,7 +16356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <f>IF(D57="","",MAX($B$4:$B56)+1)</f>
         <v>53</v>
@@ -16460,7 +16378,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <f>IF(D58="","",MAX($B$4:$B57)+1)</f>
         <v>54</v>
@@ -16498,7 +16416,7 @@
         <v>17</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16512,7 +16430,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="120" x14ac:dyDescent="0.25">
@@ -16531,13 +16449,13 @@
         <v>17</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H61" s="28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <f>IF(D62="","",MAX($B$4:$B61)+1)</f>
         <v>57</v>
@@ -16577,7 +16495,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <f>IF(D64="","",MAX($B$4:$B63)+1)</f>
         <v>59</v>
@@ -16586,14 +16504,14 @@
         <v>76</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H64" s="30" t="s">
         <v>146</v>
@@ -16615,7 +16533,7 @@
         <v>17</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>146</v>
@@ -16637,13 +16555,13 @@
         <v>17</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H66" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <f>IF(D67="","",MAX($B$4:$B66)+1)</f>
         <v>62</v>
@@ -16665,7 +16583,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <f>IF(D68="","",MAX($B$4:$B67)+1)</f>
         <v>63</v>
@@ -16687,7 +16605,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <f>IF(D69="","",MAX($B$4:$B68)+1)</f>
         <v>64</v>
@@ -16726,7 +16644,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
         <f>IF(D71="","",MAX($B$4:$B70)+1)</f>
         <v>66</v>
@@ -16735,7 +16653,7 @@
         <v>86</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
@@ -16748,7 +16666,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <f>IF(D72="","",MAX($B$4:$B71)+1)</f>
         <v>67</v>
@@ -16764,7 +16682,7 @@
         <v>136</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="195" x14ac:dyDescent="0.25">
@@ -16800,13 +16718,13 @@
         <v>17</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H74" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
         <f>IF(D75="","",MAX($B$4:$B74)+1)</f>
         <v>70</v>
@@ -16863,7 +16781,7 @@
         <v>17</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>148</v>
@@ -16878,14 +16796,14 @@
         <v>121</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H78" s="13" t="s">
         <v>147</v>
@@ -16907,7 +16825,7 @@
         <v>17</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H79" s="13" t="s">
         <v>147</v>
@@ -16935,7 +16853,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
         <f>IF(D81="","",MAX($B$4:$B80)+1)</f>
         <v>76</v>
@@ -16957,7 +16875,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="2:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
         <f>IF(D82="","",MAX($B$4:$B81)+1)</f>
         <v>77</v>
@@ -16995,7 +16913,7 @@
         <v>17</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H83" s="13" t="s">
         <v>147</v>
@@ -17017,7 +16935,7 @@
         <v>17</v>
       </c>
       <c r="G84" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H84" s="13" t="s">
         <v>147</v>
@@ -17039,7 +16957,7 @@
         <v>17</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H85" s="13" t="s">
         <v>147</v>
@@ -17054,20 +16972,20 @@
         <v>131</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H86" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="2:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
         <f>IF(D87="","",MAX($B$4:$B86)+1)</f>
         <v>82</v>
@@ -17154,7 +17072,7 @@
         <v>7</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -17188,7 +17106,7 @@
         <v>75</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
@@ -17359,12 +17277,18 @@
       <c r="G108" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:G107"/>
+  <autoFilter ref="B4:G107">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G200">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$F5="Close"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update bugs list nhung chua update code moi
</commit_message>
<xml_diff>
--- a/04_TESTING/Leakage_Bug_List.xlsx
+++ b/04_TESTING/Leakage_Bug_List.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Leakage Bug List'!$B$4:$G$106</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -10976,82 +10976,6 @@
   </si>
   <si>
     <r>
-      <t>[Tâm] retest 28/5/2012 - Passed
-Nhưng case  5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Nhập đầy đủ các field với phone đã tồn tại, click vào icon Insert -  hiện thông báo  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Can not save, change to another phone numer or UpiCode, try again later</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or contact administrator!!</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hiện tại đang dùng account của administrator thì không cần câ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>u "or contact administrator! "</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lỗi trong chức năng Insert
 </t>
     </r>
@@ -14008,23 +13932,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[Dan] Voi cach to chuc du lieu nhu hien nay ko the load len dung duoc Region, Area, Local cua Salemem. Do do phai doi schema hien tai thi moi fix duoc bug nay.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Sơn] - Hiện tại khách hàng chưa áp dụng chức năng SMSQuota và ExpiredDate cho NV Sale của họ nên việc update ExpiredDate = ngày hiện tại vẫn ok.
-Về Region, Area, Local thì chỉ áp dụng cho Customer thôi, không áp dụng cho Salesmen. Nên nếu được thì có thể áp dụng POC và POS cho Salesmen là hợp lý nhất.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">[Dan] Code hien nay da~ lay het du lieu, ko co han che, em check lai giup nhe
 </t>
     </r>
@@ -14143,6 +14050,628 @@
     </r>
   </si>
   <si>
+    <t>[Tâm] retest 29/5/2012 - Passed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Tam - 28/5/2012 ]
+1. Em chỉ nhập đúng tên của người gửi không dùng ký tự % khi search, nhưng kết quả sau khi click vào filter button thì không filter (chỉ đối với trường hợp chọn filter theo "by From" hoặc "by to" 
+2. %% ở result em để đó là điều kiện khi hiển thị kết quả mong muốn dành cho filter phải là like %String% vì like String khác với like %String%
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Dan] do du lieu bi RAC, co 1 so row co Sender name la` NULL nen code cu~ ko chay duoc =&gt; da fixed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tâm] retest 29/5/2012 - Failed
+Khi Filter theo To trong Outbox vẫn không được</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[dan] a cung ko nam ro chi biet cai table o tren dung GetManagerOfCustomer con cai table o duoi du`ng GetCustomerContact. Em co the hoi lai Son nha
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tam] Thank anh, em sẽ hỏi lại anh Sơn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Dan] anh check tren WebSite thi` thay OK mac du` ko sua gi` het. Nen em test lai giup nhe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Tam - 28/05/2012] vẫn bị anh Đan ơi
+Anh đừng nhập gì cả và click Filter button thì thấy
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] da fixed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tâm] retest 29/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
+can not add, please try again later or contact administrator! (tương tự bug 40)
+Sai ten fullname va trung so dt thi insert thanh cong
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Hien nay anh chi check Phone Number va Upi Code thoi, ko co check full name. Ful name chi check la` required field. Em verify laiu cai bug na`y giup nhe, thanks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tam] restest 29/05/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Không mở được Form khi click vào icon Edit  salesmen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repro:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   1. Login vào Account của Administrator
+   2. Click vào salesmen trên menu
+   3. Click vào icon Edit 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Result: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      Không hiện ra Form để Edit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expected: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       Show ra Form Edit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
+can not add, provide new phone number or try again later or contact asministrator. (tương tự bug 40)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Dan] Da sua message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[Tâm] retest 29/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
+can not update, please try again later or contact admnistrator. (tương tự bug 41)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] da sua msg
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Tâm] retest 29/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Dan] File dung de import phai dung dinh dang quy dinh nen ko the dung file khac de Import
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Sơn] - Không cần apply format xlsx cho chức năng này vì khách hàng không yêu cầu mình làm. Thanks all.
+[Tâm] retest 29/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
+1. Không nhập gì và click vào icon insert
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hiện câu thông báo "Please provide UPI Code and Full Name"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> câu thông báo thiếu phone number
+2. Nhập Phone number đã tồn tại vẫn insert thành công
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Dan] da sua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[Tâm] retest 29/5/2012 - Passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lỗi trong chức năng Update
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Repro:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   - Login vào Account của Administrator
+   - Click vào Customer trên menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   - Click vào icon Edit record
+    1. Xóa Full Name -&gt; click vào icon update
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Đóng Form Update lại, dữ liệu không thay đổi và chuyển xuống chờ approved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Hiện thông báo
+   2. Sửa Phone number trùng với phone number của customer khác -&gt; click vào icon update
+Result: Update thành công, chuyển xuống chờ approved
+Expected: Hiện thông báo (vì customer không thể cho trùng phone number)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Khi mất session , khi user click hiện trang báo lỗi ở một số nơi 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repro:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     Hiện ra trang lỗi "Validation of viewstate MAC failed. If this application is hosted by a Web Farm or cluster, ensure that &lt;machineKey&gt; configuration specifies the same validationKey and validation algorithm. AutoGenerate cannot be used in a cluster."
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       Khi mất session thì khi user click phải chuyển về trang default.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[Tâm] retest 28/5/2012 - Passed
+Nhưng case  5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nhập đầy đủ các field với phone đã tồn tại, click vào icon Insert -  hiện thông báo  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Can not save, change to another phone numer or UpiCode, try again later</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or contact administrator!!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hiện tại đang dùng account của administrator thì không cần câ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u "or contact administrator! "
+[Dan] administrator o day la` nguoi maintain cai site, co`n user dang nhap vo Admin chi la` nguoi quan tri noi dung site thoi</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">[Tam - 28/05/2012]
 Passed đối với filter trong Inbox
@@ -14173,80 +14702,8 @@
       </rPr>
       <t xml:space="preserve">
 [Tâm] retest 29/5/2012 - Failed
-Nhập vào textbox rối click vào clear button vẫn không reser Form Filter</t>
-    </r>
-  </si>
-  <si>
-    <t>[Tâm] retest 29/5/2012 - Passed</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Tam - 28/5/2012 ]
-1. Em chỉ nhập đúng tên của người gửi không dùng ký tự % khi search, nhưng kết quả sau khi click vào filter button thì không filter (chỉ đối với trường hợp chọn filter theo "by From" hoặc "by to" 
-2. %% ở result em để đó là điều kiện khi hiển thị kết quả mong muốn dành cho filter phải là like %String% vì like String khác với like %String%
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Dan] do du lieu bi RAC, co 1 so row co Sender name la` NULL nen code cu~ ko chay duoc =&gt; da fixed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tâm] retest 29/5/2012 - Failed
-Khi Filter theo To trong Outbox vẫn không được</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[dan] a cung ko nam ro chi biet cai table o tren dung GetManagerOfCustomer con cai table o duoi du`ng GetCustomerContact. Em co the hoi lai Son nha
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tam] Thank anh, em sẽ hỏi lại anh Sơn</t>
+Nhập vào textbox rối click vào clear button vẫn không reser Form Filter
+[Dan] da fix</t>
     </r>
   </si>
   <si>
@@ -14278,49 +14735,8 @@
 [Tam] restest 29/05/2012 - Failed
 Vẫn còn anh Đan ơi, Ví dụ:
 - Anh chọn Group -&gt; chọn Region -&gt; chọn Area -&gt; chọn Local
-- Anh chọn Group là "select"  thì chỉ có Region disabled, còn lại Area và Local thì không</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Dan] anh check tren WebSite thi` thay OK mac du` ko sua gi` het. Nen em test lai giup nhe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Tam - 28/05/2012] vẫn bị anh Đan ơi
-Anh đừng nhập gì cả và click Filter button thì thấy
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] da fixed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tâm] retest 29/5/2012 - Passed</t>
+- Anh chọn Group là "select"  thì chỉ có Region disabled, còn lại Area và Local thì không
+[dan] da fix</t>
     </r>
   </si>
   <si>
@@ -14354,181 +14770,13 @@
       <t>[Tam] restest 29/05/2012 - Failed
 Em test lại rồi nhưng ví dụ:
 - Anh chọn Group -&gt; chọn Region -&gt; chọn Area -&gt; chọn Local
-- Anh chọn Group là "select a group"  thì chỉ có Area và Local se disabled, còn lại Region thì vẫn hiện tất cả các record có trong Region, khi chọn Region thì Area sẽ được load lên</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
-can not add, please try again later or contact administrator! (tương tự bug 40)
-Sai ten fullname va trung so dt thi insert thanh cong
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Hien nay anh chi check Phone Number va Upi Code thoi, ko co check full name. Ful name chi check la` required field. Em verify laiu cai bug na`y giup nhe, thanks
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tam] restest 29/05/2012 - Passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Không mở được Form khi click vào icon Edit  salesmen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Repro:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-   1. Login vào Account của Administrator
-   2. Click vào salesmen trên menu
-   3. Click vào icon Edit 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Result: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-      Không hiện ra Form để Edit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Expected: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-       Show ra Form Edit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
-can not add, provide new phone number or try again later or contact asministrator. (tương tự bug 40)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Dan] Da sua message</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-[Tâm] retest 29/5/2012 - Passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
-can not update, please try again later or contact admnistrator. (tương tự bug 41)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] da sua msg
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Tâm] retest 29/5/2012 - Passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Dan] File dung de import phai dung dinh dang quy dinh nen ko the dung file khac de Import
+- Anh chọn Group là "select a group"  thì chỉ có Area và Local se disabled, còn lại Region thì vẫn hiện tất cả các record có trong Region, khi chọn Region thì Area sẽ được load lên
+[Dan] da sua</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Dan] Voi cach to chuc du lieu nhu hien nay ko the load len dung duoc Region, Area, Local cua Salemem. Do do phai doi schema hien tai thi moi fix duoc bug nay.
 </t>
     </r>
     <r>
@@ -14539,252 +14787,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>[Sơn] - Không cần apply format xlsx cho chức năng này vì khách hàng không yêu cầu mình làm. Thanks all.
-[Tâm] retest 29/5/2012 - Passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Tâm] retest 28/5/2012 - Failed
-1. Không nhập gì và click vào icon insert
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> hiện câu thông báo "Please provide UPI Code and Full Name"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> câu thông báo thiếu phone number
-2. Nhập Phone number đã tồn tại vẫn insert thành công
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Dan] da sua</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-[Tâm] retest 29/5/2012 - Passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lỗi trong chức năng Update
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Repro:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   - Login vào Account của Administrator
-   - Click vào Customer trên menu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-   - Click vào icon Edit record
-    1. Xóa Full Name -&gt; click vào icon update
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Đóng Form Update lại, dữ liệu không thay đổi và chuyển xuống chờ approved
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Hiện thông báo
-   2. Sửa Phone number trùng với phone number của customer khác -&gt; click vào icon update
-Result: Update thành công, chuyển xuống chờ approved
-Expected: Hiện thông báo (vì customer không thể cho trùng phone number)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Khi mất session , khi user click hiện trang báo lỗi ở một số nơi 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Repro:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-     Hiện ra trang lỗi "Validation of viewstate MAC failed. If this application is hosted by a Web Farm or cluster, ensure that &lt;machineKey&gt; configuration specifies the same validationKey and validation algorithm. AutoGenerate cannot be used in a cluster."
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-       Khi mất session thì khi user click phải chuyển về trang default.</t>
+      <t xml:space="preserve">[Sơn] - Hiện tại khách hàng chưa áp dụng chức năng SMSQuota và ExpiredDate cho NV Sale của họ nên việc update ExpiredDate = ngày hiện tại vẫn ok.
+Về Region, Area, Local thì chỉ áp dụng cho Customer thôi, không áp dụng cho Salesmen. Nên nếu được thì có thể áp dụng POC và POS cho Salesmen là hợp lý nhất.
+</t>
     </r>
   </si>
 </sst>
@@ -15130,28 +15135,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -15857,12 +15841,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:I106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15922,7 +15907,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <f>IF(D5="","",MAX($B$4:$B4)+1)</f>
         <v>1</v>
@@ -15947,7 +15932,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <f>IF(D6="","",MAX($B$4:$B5)+1)</f>
         <v>2</v>
@@ -15972,7 +15957,7 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="2:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <f>IF(D7="","",MAX($B$4:$B6)+1)</f>
         <v>3</v>
@@ -15995,7 +15980,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <f>IF(D8="","",MAX($B$4:$B7)+1)</f>
         <v>4</v>
@@ -16020,7 +16005,7 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <f>IF(D9="","",MAX($B$4:$B8)+1)</f>
         <v>5</v>
@@ -16045,7 +16030,7 @@
       </c>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f>IF(D10="","",MAX($B$4:$B9)+1)</f>
         <v>6</v>
@@ -16084,14 +16069,14 @@
         <v>17</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>60</v>
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f>IF(D12="","",MAX($B$4:$B11)+1)</f>
         <v>8</v>
@@ -16114,7 +16099,7 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <f>IF(D13="","",MAX($B$4:$B12)+1)</f>
         <v>9</v>
@@ -16137,7 +16122,7 @@
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="2:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <f>IF(D14="","",MAX($B$4:$B13)+1)</f>
         <v>10</v>
@@ -16162,7 +16147,7 @@
       </c>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="2:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f>IF(D15="","",MAX($B$4:$B14)+1)</f>
         <v>11</v>
@@ -16185,7 +16170,7 @@
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="2:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <f>IF(D16="","",MAX($B$4:$B15)+1)</f>
         <v>12</v>
@@ -16208,7 +16193,7 @@
       </c>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="240" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <f>IF(D17="","",MAX($B$4:$B16)+1)</f>
         <v>13</v>
@@ -16226,7 +16211,7 @@
         <v>17</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>56</v>
@@ -16235,7 +16220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <f>IF(D18="","",MAX($B$4:$B17)+1)</f>
         <v>14</v>
@@ -16258,7 +16243,7 @@
       </c>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="2:9" s="26" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" s="26" customFormat="1" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <f>IF(D19="","",MAX($B$4:$B18)+1)</f>
         <v>15</v>
@@ -16281,7 +16266,7 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <f>IF(D20="","",MAX($B$4:$B19)+1)</f>
         <v>16</v>
@@ -16304,7 +16289,7 @@
       </c>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <f>IF(D21="","",MAX($B$4:$B20)+1)</f>
         <v>17</v>
@@ -16327,7 +16312,7 @@
       </c>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="2:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <f>IF(D22="","",MAX($B$4:$B21)+1)</f>
         <v>18</v>
@@ -16350,7 +16335,7 @@
       </c>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <f>IF(D23="","",MAX($B$4:$B22)+1)</f>
         <v>19</v>
@@ -16373,7 +16358,7 @@
       </c>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="2:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <f>IF(D24="","",MAX($B$4:$B23)+1)</f>
         <v>20</v>
@@ -16396,7 +16381,7 @@
       </c>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="2:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <f>IF(D25="","",MAX($B$4:$B24)+1)</f>
         <v>21</v>
@@ -16419,7 +16404,7 @@
       </c>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <f>IF(D26="","",MAX($B$4:$B25)+1)</f>
         <v>22</v>
@@ -16435,14 +16420,14 @@
         <v>136</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <f>IF(D27="","",MAX($B$4:$B26)+1)</f>
         <v>23</v>
@@ -16458,7 +16443,7 @@
         <v>136</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>56</v>
@@ -16481,14 +16466,14 @@
         <v>17</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="2:9" ht="405" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <f>IF(D29="","",MAX($B$4:$B28)+1)</f>
         <v>25</v>
@@ -16504,14 +16489,14 @@
         <v>136</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="2:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <f>IF(D30="","",MAX($B$4:$B29)+1)</f>
         <v>26</v>
@@ -16534,7 +16519,7 @@
       </c>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <f>IF(D31="","",MAX($B$4:$B30)+1)</f>
         <v>27</v>
@@ -16550,14 +16535,14 @@
         <v>136</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <f>IF(D32="","",MAX($B$4:$B31)+1)</f>
         <v>28</v>
@@ -16573,14 +16558,14 @@
         <v>136</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <f>IF(D33="","",MAX($B$4:$B32)+1)</f>
         <v>29</v>
@@ -16596,14 +16581,14 @@
         <v>136</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="2:9" ht="300" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <f>IF(D34="","",MAX($B$4:$B33)+1)</f>
         <v>30</v>
@@ -16619,14 +16604,14 @@
         <v>136</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <f>IF(D35="","",MAX($B$4:$B34)+1)</f>
         <v>31</v>
@@ -16649,7 +16634,7 @@
       </c>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="2:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <f>IF(D36="","",MAX($B$4:$B35)+1)</f>
         <v>32</v>
@@ -16658,21 +16643,21 @@
         <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="2:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <f>IF(D37="","",MAX($B$4:$B36)+1)</f>
         <v>33</v>
@@ -16688,14 +16673,14 @@
         <v>136</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="2:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <f>IF(D38="","",MAX($B$4:$B37)+1)</f>
         <v>34</v>
@@ -16711,7 +16696,7 @@
         <v>136</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>56</v>
@@ -16734,14 +16719,14 @@
         <v>17</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <f>IF(D40="","",MAX($B$4:$B39)+1)</f>
         <v>36</v>
@@ -16757,14 +16742,14 @@
         <v>136</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I40" s="14"/>
     </row>
-    <row r="41" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <f>IF(D41="","",MAX($B$4:$B40)+1)</f>
         <v>37</v>
@@ -16780,14 +16765,14 @@
         <v>136</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I41" s="14"/>
     </row>
-    <row r="42" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <f>IF(D42="","",MAX($B$4:$B41)+1)</f>
         <v>38</v>
@@ -16803,14 +16788,14 @@
         <v>136</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <f>IF(D43="","",MAX($B$4:$B42)+1)</f>
         <v>39</v>
@@ -16826,13 +16811,13 @@
         <v>136</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <f>IF(D44="","",MAX($B$4:$B43)+1)</f>
         <v>40</v>
@@ -16848,13 +16833,13 @@
         <v>136</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <f>IF(D45="","",MAX($B$4:$B44)+1)</f>
         <v>41</v>
@@ -16870,13 +16855,13 @@
         <v>136</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <f>IF(D46="","",MAX($B$4:$B45)+1)</f>
         <v>42</v>
@@ -16892,13 +16877,13 @@
         <v>136</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="300" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <f>IF(D47="","",MAX($B$4:$B46)+1)</f>
         <v>43</v>
@@ -16914,13 +16899,13 @@
         <v>136</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <f>IF(D48="","",MAX($B$4:$B47)+1)</f>
         <v>44</v>
@@ -16936,13 +16921,13 @@
         <v>136</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <f>IF(D49="","",MAX($B$4:$B48)+1)</f>
         <v>45</v>
@@ -16958,13 +16943,13 @@
         <v>136</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <f>IF(D50="","",MAX($B$4:$B49)+1)</f>
         <v>46</v>
@@ -16980,13 +16965,13 @@
         <v>136</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <f>IF(D51="","",MAX($B$4:$B50)+1)</f>
         <v>47</v>
@@ -17002,13 +16987,13 @@
         <v>136</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <f>IF(D52="","",MAX($B$4:$B51)+1)</f>
         <v>48</v>
@@ -17024,13 +17009,13 @@
         <v>136</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H52" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <f>IF(D53="","",MAX($B$4:$B52)+1)</f>
         <v>49</v>
@@ -17046,13 +17031,13 @@
         <v>136</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <f>IF(D54="","",MAX($B$4:$B53)+1)</f>
         <v>50</v>
@@ -17083,20 +17068,20 @@
         <v>63</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H55" s="28" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <f>IF(D56="","",MAX($B$4:$B55)+1)</f>
         <v>52</v>
@@ -17118,7 +17103,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <f>IF(D57="","",MAX($B$4:$B56)+1)</f>
         <v>53</v>
@@ -17140,7 +17125,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <f>IF(D58="","",MAX($B$4:$B57)+1)</f>
         <v>54</v>
@@ -17178,7 +17163,7 @@
         <v>17</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17192,7 +17177,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="135" x14ac:dyDescent="0.25">
@@ -17211,13 +17196,13 @@
         <v>17</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H61" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <f>IF(D62="","",MAX($B$4:$B61)+1)</f>
         <v>57</v>
@@ -17257,7 +17242,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <f>IF(D64="","",MAX($B$4:$B63)+1)</f>
         <v>59</v>
@@ -17266,14 +17251,14 @@
         <v>76</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>145</v>
@@ -17295,7 +17280,7 @@
         <v>17</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H65" s="13" t="s">
         <v>146</v>
@@ -17317,13 +17302,13 @@
         <v>17</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="H66" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <f>IF(D67="","",MAX($B$4:$B66)+1)</f>
         <v>62</v>
@@ -17345,7 +17330,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <f>IF(D68="","",MAX($B$4:$B67)+1)</f>
         <v>63</v>
@@ -17367,7 +17352,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <f>IF(D69="","",MAX($B$4:$B68)+1)</f>
         <v>64</v>
@@ -17406,7 +17391,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
         <f>IF(D71="","",MAX($B$4:$B70)+1)</f>
         <v>66</v>
@@ -17415,7 +17400,7 @@
         <v>86</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
@@ -17428,7 +17413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <f>IF(D72="","",MAX($B$4:$B71)+1)</f>
         <v>67</v>
@@ -17444,10 +17429,10 @@
         <v>136</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <f>IF(D73="","",MAX($B$4:$B72)+1)</f>
         <v>68</v>
@@ -17463,7 +17448,7 @@
         <v>136</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H73" s="13" t="s">
         <v>146</v>
@@ -17485,13 +17470,13 @@
         <v>17</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="H74" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
         <f>IF(D75="","",MAX($B$4:$B74)+1)</f>
         <v>70</v>
@@ -17530,7 +17515,7 @@
       </c>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
         <f>IF(D77="","",MAX($B$4:$B76)+1)</f>
         <v>72</v>
@@ -17548,13 +17533,13 @@
         <v>136</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H77" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="2:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="225" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
         <f>IF(D78="","",MAX($B$4:$B77)+1)</f>
         <v>73</v>
@@ -17563,20 +17548,20 @@
         <v>121</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="H78" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
         <f>IF(D79="","",MAX($B$4:$B78)+1)</f>
         <v>74</v>
@@ -17592,7 +17577,7 @@
         <v>136</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H79" s="13" t="s">
         <v>146</v>
@@ -17614,13 +17599,13 @@
         <v>17</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="H80" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
         <f>IF(D81="","",MAX($B$4:$B80)+1)</f>
         <v>76</v>
@@ -17642,7 +17627,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="2:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
         <f>IF(D82="","",MAX($B$4:$B81)+1)</f>
         <v>77</v>
@@ -17664,7 +17649,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2">
         <f>IF(D83="","",MAX($B$4:$B82)+1)</f>
         <v>78</v>
@@ -17680,13 +17665,13 @@
         <v>136</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H83" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="2:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2">
         <f>IF(D84="","",MAX($B$4:$B83)+1)</f>
         <v>79</v>
@@ -17702,13 +17687,13 @@
         <v>136</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H84" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
         <f>IF(D85="","",MAX($B$4:$B84)+1)</f>
         <v>80</v>
@@ -17724,13 +17709,13 @@
         <v>17</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H85" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
         <f>IF(D86="","",MAX($B$4:$B85)+1)</f>
         <v>81</v>
@@ -17739,20 +17724,20 @@
         <v>131</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H86" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="2:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
         <f>IF(D87="","",MAX($B$4:$B86)+1)</f>
         <v>82</v>
@@ -17774,7 +17759,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2">
         <f>IF(D88="","",MAX($B$4:$B87)+1)</f>
         <v>83</v>
@@ -17790,7 +17775,7 @@
         <v>136</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>145</v>
@@ -17813,7 +17798,7 @@
       </c>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
         <f>IF(D90="","",MAX($B$4:$B89)+1)</f>
         <v>85</v>
@@ -17830,7 +17815,7 @@
       </c>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="2:8" ht="390" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
         <f>IF(D91="","",MAX($B$4:$B90)+1)</f>
         <v>86</v>
@@ -17839,7 +17824,7 @@
         <v>7</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -17847,7 +17832,7 @@
       </c>
       <c r="G91" s="7"/>
     </row>
-    <row r="92" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
         <f>IF(D92="","",MAX($B$4:$B91)+1)</f>
         <v>87</v>
@@ -17873,7 +17858,7 @@
         <v>75</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
@@ -17890,7 +17875,7 @@
         <v>121</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
@@ -17907,7 +17892,7 @@
         <v>131</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
@@ -17922,7 +17907,7 @@
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -18039,7 +18024,13 @@
       <c r="G106" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:G106"/>
+  <autoFilter ref="B4:G106">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>

</xml_diff>